<commit_message>
Modified to handle missing values and wrong output values
</commit_message>
<xml_diff>
--- a/extracted_data.xlsx
+++ b/extracted_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,35 +446,50 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>City</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Domain</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Branches</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Accomodation</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Timings</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Weekly Holidays</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Stipend for Single Degree</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Tech skills</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Non Tech skills</t>
         </is>
@@ -482,226 +497,301 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>6636</v>
+        <v>6865</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>505 Army Base Workshop-Electro Mechanics</t>
+          <t>505 Army Base Workshop-CS/IT</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>A3, A4, A8, AA</t>
+          <t>Delhi</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>Delhi</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Mechanical</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>A7</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>9:00 AM to 2:00 PM</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Sunday</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>sunday</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Electronics,Mechanical Processes,Mechanical &amp; Electrical forces on Transformers,Mechanical,Knowledge of key Mechanical Equipment</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Analytical Skill,Excellent communication</t>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Software Development</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Analytical Skill</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>6686</v>
+        <v>6636</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>83 D Network Private Limited</t>
+          <t>505 Army Base Workshop-Electro Mechanics</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>A7</t>
+          <t>New Delhi</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>Delhi</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Electronics</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>A3, A4, A8, AA</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>9:00 AM to 6:00 PM</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Saturday, Sunday</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>9:00 AM to 2:00 PM</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>sunday</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>#NA</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t># NA</t>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Electronics,Mechanical Processes,Mechanical &amp; Electrical forces on Transformers,Mechanical,Knowledge of key Mechanical Equipment</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Analytical Skill,Excellent communication</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>6790</v>
+        <v>6846</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Adani Solar - Mundra Solar Private Limited</t>
+          <t>505 Army Base Workshop-Manufacturing</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>A1, A2, A3, A4, A5, A7, A8, AA, AB, B1, B2, B3, B4, B5, C2, C6, C7, D2</t>
+          <t>New Delhi</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>Delhi</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Manufacturing</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>A4, AB</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>9:00 AM to 6:00 PM</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Sunday</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>9:00 AM to 2:00 PM</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>sunday</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>#NA</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t># NA</t>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Mechanical Processes,Mechanical,Manufacturing,Manufacturing &amp; Materials,Manufacturing Operation Tools</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Analytical Skill</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>6753</v>
+        <v>6845</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Advanced Systems Laboratory, DRDO</t>
+          <t>505 Army Base Workshop-Mechanical</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>A3, A8, AA</t>
+          <t>New Delhi</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>Delhi</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Electronics</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>A4</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>9:00 AM to 5:00 PM</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Sunday</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>9:00 AM to 2:00 PM</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>sunday</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>#NA</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Communication Skill,Analytical Skill</t>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Mechanical,Mechanical &amp; Electrical forces on Transformers</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Analytical Skill</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>6722</v>
+        <v>6866</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>AGATSYA EDUTECH PRIVATE LIMITED</t>
+          <t>505 Army Base Workshop-Mechatronics</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>A1, A2, A3, A4, A5, A7, A8, AA, AB, B1, B2, B3, B4, B5, C2, C6, C7, D2</t>
+          <t>Delhi</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
+          <t>Delhi</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Mechanical</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>A4, A7, A8, AA</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>10:00 AM to 7:00 PM</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Sunday</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>9:00 AM to 2:00 PM</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>sunday</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Photoshop and Design experience</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Communication Skill,Analytical Skill</t>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Mechanical,Mechanical &amp; Electrical forces on Transformers,Mechanical Processes</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Analytical Skill</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated to get project name description
</commit_message>
<xml_diff>
--- a/extracted_data.xlsx
+++ b/extracted_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,6 +494,16 @@
           <t>Non Tech skills</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Project Title</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Project Description</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -511,7 +521,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Delhi</t>
+          <t>India</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -552,6 +562,24 @@
       <c r="L2" t="inlineStr">
         <is>
           <t>Analytical Skill</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Production management software for Army Base Workshop</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Production management software for Army Base Workshop
+Project Description
+Description: 
+A. Existing setup : The OH of a tank is a 6 stage process spread over 144 days. It involves multiple entities working in tandem to achieve the target in time.
+B. Problem Statement :
+1. Development of a software application/ package to monitor the progress of production process.
+2. The software should be able to identify crucial bottlenecks and suggest corrective action in advance
+3. assist in easy HR management
+Skill sets : Proficiency in programming languages, data structures, algorithms, problem solving and communication</t>
         </is>
       </c>
     </row>
@@ -571,7 +599,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Delhi</t>
+          <t>India</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -612,6 +640,26 @@
       <c r="L3" t="inlineStr">
         <is>
           <t>Analytical Skill,Excellent communication</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Engine Health Monitoring System.</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Engine Health Monitoring System.
+Project Description
+Existing Setup : Instantaneous and not continuous monitoring, leads to reactive maintenance than preventive maintenance.
+Problem Statement.
+(i) Analog System to be digitized.
+(ii) Requirement of ECU that takes input from all sensors.
+(iii) Deviation of critical engine parameters from normal to be logged and highlighted.
+(iv) Pin-point fault diagnosis.
+(v) Predict and alert for preventive maintenance in advance.
+(vi) Remote Diagnosis of Faults.
+Skill Sets: Electro Mechanics</t>
         </is>
       </c>
     </row>
@@ -631,7 +679,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Delhi</t>
+          <t>India</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -666,12 +714,35 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Mechanical Processes,Mechanical,Manufacturing,Manufacturing &amp; Materials,Manufacturing Operation Tools</t>
+          <t>Manufacturing,Manufacturing Operation Tools,Mechanical,Mechanical Processes</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
           <t>Analytical Skill</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Title:Re-manufacturing of certain internal components for reduction in weight thereby improving power to weight ratio.</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Title:Re-manufacturing of certain internal components for reduction in weight thereby improving power to weight ratio.
+Project Description
+Description:
+(a) Existing Setup: Metallic parts designed for ruggedness.
+Therefore, they are bulky and reduce the power to weight ratio.
+Additionally, the fuel/ammunition within is susceptible to catching fire
+and even exploding due to enemy fire.
+(b) Problem Statement: Finding suitable alternative material for .
+re-manufacturing these components such that the new component is:-
+(i) Light Weight-leading to increase in power to weight ratio.
+(ii) Self Sealing in cases where fuel/oils/lubricants are contained
+within.
+(iii) Blast proof stowage for ammunition.
+Skill Sets: Mechanical</t>
         </is>
       </c>
     </row>
@@ -691,7 +762,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Delhi</t>
+          <t>India</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -732,6 +803,22 @@
       <c r="L5" t="inlineStr">
         <is>
           <t>Analytical Skill</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Re-designing of external components for reduction in thermal signature, thereby enhancing Tank protection.</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Re-designing of external components for reduction in thermal signature, thereby enhancing Tank protection.
+Project Description
+Description:
+(a) Existing Setup. Entirely metallic, designed ruggedness.
+(b) Problem Statement. Finding suitable alternative
+technology for reducing the external heat signature of the Tank.
+Skill Sets:MechanicaI, Machine Design</t>
         </is>
       </c>
     </row>
@@ -751,7 +838,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Delhi</t>
+          <t>India</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -792,6 +879,29 @@
       <c r="L6" t="inlineStr">
         <is>
           <t>Analytical Skill</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>lndigenization of Induction Sensor of PWDM and Potentiometer (HYDR1 )</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>lndigenization of Induction Sensor of PWDM and Potentiometer (HYDR1 )
+Project Description
+Description:
+(a) Existing Setup: Both are essential for Turret Traverse in Stab
+and non Stab mode and not available through Ordnance channel.
+(b) Problem Statement:-
+(i) Not available in normal source of supply.
+(ii) UNSV in over hauling of Tanks.
+(iii) Required 01(potentiometer (HYDR1)) and 02 (Induction
+Sensor) qty per Tank.
+(iv) Not developed by BEL.
+(v) Ex-import spare.
+(vi) Local Vendor/Supplier is not available.
+Skill Sets:- Electro Mechanics</t>
         </is>
       </c>
     </row>

</xml_diff>